<commit_message>
Updated tiny talon to RF4.2.9. Update calc for swash angle.
</commit_message>
<xml_diff>
--- a/Swash angle calc.xlsx
+++ b/Swash angle calc.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="27">
   <si>
     <t># rules    i  OP SRC DST WEIGHT OFFSET MODES</t>
   </si>
   <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t>Phase angle</t>
   </si>
   <si>
@@ -93,6 +90,21 @@
   </si>
   <si>
     <t xml:space="preserve"> add </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevator servo Position </t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Rear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -146,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -342,11 +354,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -391,6 +440,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:H27"/>
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +752,11 @@
     <col min="19" max="22" width="4.7109375" customWidth="1"/>
     <col min="23" max="23" width="6.7109375" style="12" customWidth="1"/>
     <col min="24" max="24" width="6.7109375" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -723,14 +783,18 @@
       <c r="X1" s="17"/>
       <c r="Y1" s="19"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
+      <c r="B2" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="E2" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
@@ -749,17 +813,16 @@
       <c r="W2" s="22"/>
       <c r="X2" s="21"/>
       <c r="Y2" s="23"/>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
-        <v>12</v>
-      </c>
+      <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
@@ -780,15 +843,20 @@
       <c r="W3" s="22"/>
       <c r="X3" s="21"/>
       <c r="Y3" s="23"/>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="10">
-        <v>0</v>
+      <c r="B4" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="E4" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
       <c r="H4" s="21"/>
@@ -810,9 +878,11 @@
       <c r="X4" s="21"/>
       <c r="Y4" s="23"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -836,8 +906,15 @@
       <c r="W5" s="22"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="23"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA5">
+        <v>1000</v>
+      </c>
+      <c r="AB5">
+        <f>IF(E$2=$AA$2,AA5,AA5*-1)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -863,12 +940,17 @@
       <c r="W6" s="22"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="23"/>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>-500</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB8" si="0">IF(E$2=$AA$2,AA6,AA6*-1)</f>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="B7" s="21" t="s">
-        <v>8</v>
-      </c>
+      <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -876,9 +958,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="21" t="s">
-        <v>9</v>
-      </c>
+      <c r="J7" s="21"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -886,9 +966,7 @@
       <c r="O7" s="22"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
-      <c r="R7" s="21" t="s">
-        <v>10</v>
-      </c>
+      <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
@@ -896,79 +974,92 @@
       <c r="W7" s="22"/>
       <c r="X7" s="21"/>
       <c r="Y7" s="23"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <v>-766</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="0"/>
+        <v>-766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="23"/>
+      <c r="AA8">
+        <v>-707</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="0"/>
+        <v>-707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="2" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="2" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="23"/>
-      <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="7"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="4"/>
       <c r="Y9" s="23"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -978,7 +1069,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="21"/>
       <c r="J10" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -988,7 +1079,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -999,386 +1090,350 @@
       <c r="Y10" s="23"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="14">
-        <v>500</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="21"/>
       <c r="J11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O11" s="14">
-        <v>500</v>
-      </c>
-      <c r="P11" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="21"/>
       <c r="R11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="W11" s="14">
-        <v>500</v>
-      </c>
-      <c r="X11" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="7"/>
       <c r="Y11" s="23"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="14">
         <v>500</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>20</v>
+      <c r="H12" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O12" s="14">
         <v>500</v>
       </c>
       <c r="P12" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q12" s="21"/>
       <c r="R12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="W12" s="14">
         <v>500</v>
       </c>
       <c r="X12" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y12" s="23"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" s="14">
         <v>500</v>
       </c>
-      <c r="H13" s="30" t="s">
-        <v>20</v>
+      <c r="H13" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="6">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="6">
-        <v>2</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="M13" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O13" s="14">
         <v>500</v>
       </c>
       <c r="P13" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q13" s="21"/>
       <c r="R13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="6">
+        <v>1</v>
+      </c>
+      <c r="T13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S13" s="6">
-        <v>2</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="U13" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W13" s="14">
         <v>500</v>
       </c>
       <c r="X13" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y13" s="23"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="14">
+        <v>500</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="I14" s="21"/>
       <c r="J14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="K14" s="6">
+        <v>2</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="14">
+        <v>500</v>
+      </c>
+      <c r="P14" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Q14" s="21"/>
       <c r="R14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="S14" s="6">
+        <v>2</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W14" s="14">
+        <v>500</v>
+      </c>
+      <c r="X14" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Y14" s="23"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6">
         <v>3</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="14">
-        <v>866</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>20</v>
-      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="21"/>
       <c r="J15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="6">
         <v>3</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O15" s="14">
-        <v>643</v>
-      </c>
-      <c r="P15" s="30" t="s">
-        <v>20</v>
-      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="30"/>
       <c r="Q15" s="21"/>
       <c r="R15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S15" s="6">
         <v>3</v>
       </c>
-      <c r="T15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="W15" s="14">
-        <v>707</v>
-      </c>
-      <c r="X15" s="30" t="s">
-        <v>20</v>
-      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="30"/>
       <c r="Y15" s="23"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" s="14">
-        <v>-866</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>20</v>
+        <v>866</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K16" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O16" s="14">
-        <v>-643</v>
+        <v>643</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16" s="21"/>
       <c r="R16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S16" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V16" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W16" s="14">
-        <v>-707</v>
+        <v>707</v>
       </c>
       <c r="X16" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y16" s="23"/>
       <c r="AA16" s="1"/>
@@ -1386,732 +1441,819 @@
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="14">
+        <v>-866</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>26</v>
+      </c>
       <c r="I17" s="21"/>
       <c r="J17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="K17" s="6">
+        <v>4</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="14">
+        <v>-643</v>
+      </c>
+      <c r="P17" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Q17" s="21"/>
       <c r="R17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="S17" s="6">
+        <v>4</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W17" s="14">
+        <v>-707</v>
+      </c>
+      <c r="X17" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Y17" s="23"/>
       <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="6">
-        <v>5</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="14">
-        <v>1000</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="35"/>
       <c r="I18" s="21"/>
       <c r="J18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="6">
-        <v>5</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O18" s="14">
-        <v>1000</v>
-      </c>
-      <c r="P18" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="30"/>
       <c r="Q18" s="21"/>
       <c r="R18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S18" s="6">
-        <v>5</v>
-      </c>
-      <c r="T18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="W18" s="14">
-        <v>1000</v>
-      </c>
-      <c r="X18" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="30"/>
       <c r="Y18" s="23"/>
       <c r="AA18" s="1"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="G19" s="14">
-        <v>-500</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>20</v>
+        <f>AB5</f>
+        <v>1000</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N19" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="O19" s="14">
-        <v>-766</v>
+        <f>AB5</f>
+        <v>1000</v>
       </c>
       <c r="P19" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q19" s="21"/>
       <c r="R19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S19" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="V19" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="W19" s="14">
-        <v>-707</v>
+        <f>AB5</f>
+        <v>1000</v>
       </c>
       <c r="X19" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y19" s="23"/>
+      <c r="AA19" s="1"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" s="14">
+        <f>AB6</f>
         <v>-500</v>
       </c>
-      <c r="H20" s="30" t="s">
-        <v>20</v>
+      <c r="H20" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="I20" s="21"/>
       <c r="J20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K20" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O20" s="14">
+        <f>AB7</f>
         <v>-766</v>
       </c>
       <c r="P20" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q20" s="21"/>
       <c r="R20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S20" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V20" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W20" s="14">
+        <f>AB8</f>
         <v>-707</v>
       </c>
       <c r="X20" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y20" s="23"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="14">
+        <f>G20</f>
+        <v>-500</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>26</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="K21" s="6">
+        <v>7</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O21" s="14">
+        <f>O20</f>
+        <v>-766</v>
+      </c>
+      <c r="P21" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Q21" s="21"/>
       <c r="R21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="S21" s="6">
+        <v>7</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W21" s="14">
+        <f>W20</f>
+        <v>-707</v>
+      </c>
+      <c r="X21" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Y21" s="23"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="6">
-        <v>8</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="14">
-        <f>TAN(RADIANS($B$4))*G18</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="21"/>
       <c r="J22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="6">
-        <v>8</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O22" s="14">
-        <f>TAN(RADIANS($B$4))*O18</f>
-        <v>0</v>
-      </c>
-      <c r="P22" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="30"/>
       <c r="Q22" s="21"/>
       <c r="R22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="6">
-        <v>8</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="W22" s="14">
-        <f>TAN(RADIANS($B$4))*W18</f>
-        <v>0</v>
-      </c>
-      <c r="X22" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="30"/>
       <c r="Y22" s="23"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G23" s="14">
-        <f>TAN(RADIANS($B$4))*G19</f>
+        <f>TAN(RADIANS($B$5))*G19</f>
         <v>0</v>
       </c>
-      <c r="H23" s="30" t="s">
-        <v>20</v>
+      <c r="H23" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O23" s="14">
-        <f>TAN(RADIANS($B$4))*O19</f>
+        <f>TAN(RADIANS($B$5))*O19</f>
         <v>0</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q23" s="21"/>
       <c r="R23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S23" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V23" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="W23" s="14">
-        <f>TAN(RADIANS($B$4))*W19</f>
+        <f>TAN(RADIANS($B$5))*W19</f>
         <v>0</v>
       </c>
       <c r="X23" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y23" s="23"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G24" s="14">
-        <f>TAN(RADIANS($B$4))*G20</f>
+        <f>TAN(RADIANS($B$5))*G20</f>
         <v>0</v>
       </c>
-      <c r="H24" s="30" t="s">
-        <v>20</v>
+      <c r="H24" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O24" s="14">
-        <f>TAN(RADIANS($B$4))*O20</f>
+        <f>TAN(RADIANS($B$5))*O20</f>
         <v>0</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="21"/>
       <c r="R24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S24" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V24" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W24" s="14">
-        <f>TAN(RADIANS($B$4))*W20</f>
+        <f>TAN(RADIANS($B$5))*W20</f>
         <v>0</v>
       </c>
       <c r="X24" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y24" s="23"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="6">
+        <v>10</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="14">
+        <f>TAN(RADIANS($B$5))*G21</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>26</v>
+      </c>
       <c r="I25" s="21"/>
       <c r="J25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="K25" s="6">
+        <v>10</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O25" s="14">
+        <f>TAN(RADIANS($B$5))*O21</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Q25" s="21"/>
       <c r="R25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="S25" s="6">
+        <v>10</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W25" s="14">
+        <f>TAN(RADIANS($B$5))*W21</f>
+        <v>0</v>
+      </c>
+      <c r="X25" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="Y25" s="23"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="6">
-        <v>11</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="14">
-        <f>TAN(RADIANS($B$4))*G15</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="21"/>
       <c r="J26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="6">
-        <v>11</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" s="14">
-        <f>TAN(RADIANS($B$4))*O15</f>
-        <v>0</v>
-      </c>
-      <c r="P26" s="30" t="s">
-        <v>20</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="30"/>
       <c r="Q26" s="21"/>
       <c r="R26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="6">
+        <v>6</v>
+      </c>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="23"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="6">
         <v>11</v>
       </c>
-      <c r="T26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U26" s="6" t="s">
+      <c r="D27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="V26" s="6" t="s">
+      <c r="G27" s="14">
+        <f>TAN(RADIANS($B$5))*G16</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="21"/>
+      <c r="J27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="6">
+        <v>11</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="14">
+        <f>TAN(RADIANS($B$5))*O16</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="6">
+        <v>11</v>
+      </c>
+      <c r="T27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="W27" s="14">
+        <f>TAN(RADIANS($B$5))*W16</f>
+        <v>0</v>
+      </c>
+      <c r="X27" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y27" s="23"/>
+    </row>
+    <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="9">
+        <v>12</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W26" s="14">
-        <f>TAN(RADIANS($B$4))*W15</f>
+      <c r="G28" s="15">
+        <f>TAN(RADIANS($B$5))*G17</f>
         <v>0</v>
       </c>
-      <c r="X26" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y26" s="23"/>
-    </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="9">
-        <v>12</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="15">
-        <f>TAN(RADIANS($B$4))*G16</f>
+      <c r="H28" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="21"/>
+      <c r="J28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="9">
+        <v>12</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="15">
+        <f>TAN(RADIANS($B$5))*O17</f>
         <v>0</v>
       </c>
-      <c r="H27" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="9">
-        <v>12</v>
-      </c>
-      <c r="L27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O27" s="15">
-        <f>TAN(RADIANS($B$4))*O16</f>
+      <c r="P28" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S28" s="9">
+        <v>12</v>
+      </c>
+      <c r="T28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="U28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W28" s="15">
+        <f>TAN(RADIANS($B$5))*W17</f>
         <v>0</v>
       </c>
-      <c r="P27" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="S27" s="9">
-        <v>12</v>
-      </c>
-      <c r="T27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="U27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="V27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="W27" s="15">
-        <f>TAN(RADIANS($B$4))*W16</f>
-        <v>0</v>
-      </c>
-      <c r="X27" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y27" s="23"/>
-    </row>
-    <row r="28" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="21"/>
+      <c r="X28" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="Y28" s="23"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="29"/>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+    <row r="29" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="23"/>
+    </row>
+    <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="29"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:G2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G2">
+      <formula1>$AA$2:$AA$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>